<commit_message>
Add Privacy page with navigation and footer links
- Added Privacy link to navigation between Premium and About
- Created new Privacy page at /privacy with comprehensive privacy sections:
  - Secure by Design (TLS encryption, E2E roadmap)
  - Zero Human Access (no data review/selling)
  - Transparent Infrastructure (U.S. cloud, audited centers)
  - Full Export & Deletion Control
  - No Data Monetization (subscription model)
  - Our Commitment
- Updated PrivacySection on homepage with link to Privacy Overview
- Fixed Footer Privacy link to point to /privacy instead of homepage anchor
- Matched styling with About page (Cards, font-mono, consistent spacing)

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/docs/MindMirror_Marketing.xlsx
+++ b/docs/MindMirror_Marketing.xlsx
@@ -4,18 +4,20 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Outreach" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Copywrites" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="ICP" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Sample" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="Copywrites 1st msg" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Reddit DMs" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="Followup msgs" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="ICP" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="Sample" sheetId="6" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Outreach!$A$1:$J$27</definedName>
-    <definedName hidden="1" localSheetId="3" name="_xlnm._FilterDatabase">Sample!$A$1:$H$4</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Outreach!$A$1:$J$32</definedName>
+    <definedName hidden="1" localSheetId="5" name="_xlnm._FilterDatabase">Sample!$A$1:$H$4</definedName>
   </definedNames>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataChecksum="H2MhdUy67vFC81HMLEvjme+KlgBYC4qGL8QzZ40iAkk="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId10" roundtripDataChecksum="qzajpeeLuoBf6BjqMsoSghMdJ06MskDHULm3M8DAzp0="/>
     </ext>
   </extLst>
 </workbook>
@@ -51,6 +53,24 @@
 ======</t>
       </text>
     </comment>
+    <comment authorId="0" ref="F22">
+      <text>
+        <t xml:space="preserve">waiting for his message, otherwise followup with Misha dubai
+======</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="A28">
+      <text>
+        <t xml:space="preserve">Building LLM agents 
+======</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="A29">
+      <text>
+        <t xml:space="preserve"> From Oli In Finance Zurich
+======</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="G15">
       <text>
         <t xml:space="preserve">======
@@ -59,7 +79,7 @@
 uses Claude Code, not building AI agents</t>
       </text>
     </comment>
-    <comment authorId="0" ref="G25">
+    <comment authorId="0" ref="G26">
       <text>
         <t xml:space="preserve">======
 ID#AAABsCcTdwg
@@ -77,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="163">
   <si>
     <t>Name</t>
   </si>
@@ -190,6 +210,9 @@
     <t>Jarvis AI hobbyist</t>
   </si>
   <si>
+    <t>Discord</t>
+  </si>
+  <si>
     <t>Low</t>
   </si>
   <si>
@@ -235,6 +258,9 @@
     <t>Misha (Dubai)</t>
   </si>
   <si>
+    <t>Misha (Dubai) Friend</t>
+  </si>
+  <si>
     <t>Matteo TechLabs</t>
   </si>
   <si>
@@ -244,6 +270,9 @@
     <t>YouTube DM</t>
   </si>
   <si>
+    <t>Maybe</t>
+  </si>
+  <si>
     <t>Ruslan Gafarov</t>
   </si>
   <si>
@@ -256,7 +285,19 @@
     <t>Artem Ira Rostov</t>
   </si>
   <si>
-    <t>Maybe</t>
+    <t>Grigoriy Crypto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nikita from Darina </t>
+  </si>
+  <si>
+    <t>‪+380 97 336 9308‬</t>
+  </si>
+  <si>
+    <t>Nic Macerola AI/IT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valekh </t>
   </si>
   <si>
     <t>GPT lovers group</t>
@@ -291,7 +332,7 @@
   <si>
     <t>– Привет, как дела?
 – …
-– Супер. Слушай, я буквально на пару минут. Я сделал инструмент, который решает проблему у ИИ с памятью. Например, ChatGPT помнит только внутри одного чата, а открыл новый — всё забывает. Я добавил систему, которая даёт Клоду постоянную память через MCP протокол.
+– Супер. Слушай, я буквально на пару минут. Я сделал инструмент, который решает проблему у ИИ с памятью. Например, ChatGPT помнит только внутри одного чата, а открыл новый - всё забывает. Я добавил систему, которая даёт Клоду постоянную память через MCP протокол.
 – Это в первую очередь для разработчиков, которые строят агентов, но и обычные пользователи Клода могут использовать. Бесплатно до 25 «памятей».
 – Я знаю, ты больше в финансах/крипте, может быть тебе самому это не супер актуально. Но, может, у тебя есть знакомые в IT/AI, кому это реально полезно? Потенциальные пользователи, талантливые ребята, может даже те, кого можно затащить в проект как сотрудников или партнёров.
 – Если можешь меня с ними связать, было бы очень круто.</t>
@@ -332,7 +373,7 @@
     <t>Email</t>
   </si>
   <si>
-    <t>Subject: Quick favor — try what I built?
+    <t>Subject: Quick favor - try what I built?
 Hey [Name],
 I built a tool that gives AI chats memory (keeps context across sessions).
 It’s free up to 25 memories.
@@ -340,6 +381,177 @@
 www.usemindmirror.com
 Thanks,
 Artem</t>
+  </si>
+  <si>
+    <t>Example DM System</t>
+  </si>
+  <si>
+    <t>Pipeline logic (print this in your brain)</t>
+  </si>
+  <si>
+    <t>Contact volume first</t>
+  </si>
+  <si>
+    <t>Qualification second</t>
+  </si>
+  <si>
+    <t>Personalization third</t>
+  </si>
+  <si>
+    <t>Follow-up fourth</t>
+  </si>
+  <si>
+    <t>Base DM:</t>
+  </si>
+  <si>
+    <t>Demo/onboarding last</t>
+  </si>
+  <si>
+    <t>Hey, saw your comment in the Memori thread — you seem to be working with AI memory/state stuff. Curious, are you building anything right now with Claude or AI agents?</t>
+  </si>
+  <si>
+    <t>Personalization tweak (1 line only):</t>
+  </si>
+  <si>
+    <t>If they mention embeddings →</t>
+  </si>
+  <si>
+    <t>“Saw your comment about embeddings/appending context, good point.”</t>
+  </si>
+  <si>
+    <t>If they talk about LiteLLM →</t>
+  </si>
+  <si>
+    <t>“You’re right about LiteLLM dependency issues btw.”</t>
+  </si>
+  <si>
+    <t>If they talk about architecture →</t>
+  </si>
+  <si>
+    <t>“Interesting how you think about memory architecture.”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">u can dm everyone under certain posts follow up only with med and high ICP </t>
+  </si>
+  <si>
+    <t>🎯 Classification rules for commenters:</t>
+  </si>
+  <si>
+    <t>When someone replies, classify immediately:</t>
+  </si>
+  <si>
+    <t>Response Type</t>
+  </si>
+  <si>
+    <t>ICP Status</t>
+  </si>
+  <si>
+    <t>Track in Excel?</t>
+  </si>
+  <si>
+    <t>Follow-up?</t>
+  </si>
+  <si>
+    <t>Clearly building AI agents/tools</t>
+  </si>
+  <si>
+    <t>✅ High ICP</t>
+  </si>
+  <si>
+    <t>✅ Yes</t>
+  </si>
+  <si>
+    <t>AI dev / indie hacker / automation guy</t>
+  </si>
+  <si>
+    <t>✅ Medium ICP</t>
+  </si>
+  <si>
+    <t>Curious commenter (no projects)</t>
+  </si>
+  <si>
+    <t>❌ Low ICP</t>
+  </si>
+  <si>
+    <t>❌ No</t>
+  </si>
+  <si>
+    <t>Philosopher/troll/smartass</t>
+  </si>
+  <si>
+    <t>❌ Ignore</t>
+  </si>
+  <si>
+    <t>Helpful expert but not ICP</t>
+  </si>
+  <si>
+    <t>🔁 Referral ICP</t>
+  </si>
+  <si>
+    <t>Maybe if useful</t>
+  </si>
+  <si>
+    <t>1 follow-up max</t>
+  </si>
+  <si>
+    <t>Follow-up #1 (after 2–3 days):</t>
+  </si>
+  <si>
+    <t>Hey, did you get a chance to try MindMirror yet? No rush - just curious if it works for your setup or not.</t>
+  </si>
+  <si>
+    <t>If they still don’t reply after 2–3 more days:</t>
+  </si>
+  <si>
+    <t>Follow-up #2 (low friction):</t>
+  </si>
+  <si>
+    <t>If you’re busy, all good - just tell me: should I</t>
+  </si>
+  <si>
+    <t>A) remind you later</t>
+  </si>
+  <si>
+    <t>B) send setup instructions</t>
+  </si>
+  <si>
+    <t>C) leave you alone 😄</t>
+  </si>
+  <si>
+    <t>What to do with low-ICP people who replied “I’ll see what I can do"</t>
+  </si>
+  <si>
+    <t>Thanks, appreciate it 🙌 If anyone comes to mind later, just let me know.</t>
+  </si>
+  <si>
+    <t>No worries 🙌 If anyone comes to mind later, just let me know. 😁</t>
+  </si>
+  <si>
+    <t>For devs/technical users, here’s a tailored version:</t>
+  </si>
+  <si>
+    <t>Dev follow-up:</t>
+  </si>
+  <si>
+    <t>Did you get a chance to connect MindMirror to Claude via MCP yet? Curious if it actually solves anything for you or not.</t>
+  </si>
+  <si>
+    <t>And if someone said they’ll try but disappeared:</t>
+  </si>
+  <si>
+    <t>Accountability follow-up:</t>
+  </si>
+  <si>
+    <t>Still planning to test it or should I cross you off? No hard feelings either way.</t>
+  </si>
+  <si>
+    <t>If you want a referral-focused follow-up:</t>
+  </si>
+  <si>
+    <t>Referral follow-up:</t>
+  </si>
+  <si>
+    <t>Even if you’re not using it yourself, maybe you know someone building AI agents or working with Claude who might want this? One intro would really help.</t>
   </si>
   <si>
     <t>MindMirror ICP
@@ -512,15 +724,25 @@
       <t xml:space="preserve"> → Contacted, not useful, don't chase</t>
     </r>
   </si>
+  <si>
+    <t xml:space="preserve">High = Direct users - devs/AI builders who would use MindMirror themselves
+(Examples: Ismail, Damian, Semyon, Ahmed MCP guy)
+Medium = Tech-curious or referral connectors - may know devs or could refer
+(Examples: Gaia, Ivan TASIS, Nastya, your classmates who might know devs)
+Low = General friends/community - not technical but might spread the word
+(Examples: TASIS WhatsApp group, Jarvis AI hobbyist)
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d\ mmm"/>
+    <numFmt numFmtId="165" formatCode="d mmm"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="18">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -577,6 +799,55 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF0E0E0E"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -592,7 +863,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="30">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -607,6 +878,12 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
@@ -616,7 +893,7 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
@@ -625,6 +902,30 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -648,6 +949,14 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -1118,52 +1427,52 @@
       <c r="B13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>27</v>
+      <c r="C13" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G13" s="5"/>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G14" s="5"/>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F15" s="4">
         <v>45940.0</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>9</v>
@@ -1172,41 +1481,46 @@
         <v>34</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="5"/>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>34</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F17" s="4">
         <v>45940.0</v>
       </c>
-      <c r="G17" s="5"/>
+      <c r="G17" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" s="8">
+        <v>45946.0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F18" s="4">
         <v>45940.0</v>
@@ -1215,7 +1529,7 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>9</v>
@@ -1224,7 +1538,7 @@
         <v>34</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F19" s="4">
         <v>45940.0</v>
@@ -1233,7 +1547,7 @@
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>32</v>
@@ -1242,7 +1556,7 @@
         <v>15</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F20" s="4">
         <v>45940.0</v>
@@ -1251,7 +1565,7 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>9</v>
@@ -1260,7 +1574,7 @@
         <v>15</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F21" s="4">
         <v>45940.0</v>
@@ -1268,53 +1582,57 @@
       <c r="G21" s="5"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22" s="2" t="s">
+      <c r="A22" s="6" t="s">
         <v>53</v>
       </c>
+      <c r="B22" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="C22" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F22" s="4">
-        <v>45940.0</v>
-      </c>
-      <c r="G22" s="5"/>
+        <v>15</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="4"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="8"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="C23" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>44</v>
+        <v>56</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="F23" s="4">
         <v>45940.0</v>
       </c>
-      <c r="G23" s="5"/>
+      <c r="G23" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H23" s="8">
+        <v>45946.0</v>
+      </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F24" s="4">
         <v>45940.0</v>
@@ -1323,59 +1641,144 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>9</v>
+        <v>60</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F25" s="4">
         <v>45940.0</v>
       </c>
-      <c r="G25" s="2" t="s">
-        <v>59</v>
-      </c>
+      <c r="G25" s="5"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="7" t="s">
-        <v>60</v>
+      <c r="A26" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E26" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G26" s="5"/>
+      <c r="E26" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F26" s="4">
+        <v>45940.0</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="G27" s="5"/>
-      <c r="J27" s="2" t="s">
-        <v>61</v>
+      <c r="A27" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" s="4">
+        <v>45940.0</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H27" s="8">
+        <v>45949.0</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
+      <c r="A28" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="8">
+        <v>45946.0</v>
+      </c>
       <c r="G28" s="5"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
+      <c r="A29" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F29" s="9">
+        <v>45947.0</v>
+      </c>
       <c r="G29" s="5"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="G30" s="5"/>
+      <c r="A30" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="9">
+        <v>45948.0</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
+      <c r="A31" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>45</v>
+      </c>
       <c r="G31" s="5"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="G32" s="5"/>
+      <c r="J32" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="G33" s="5"/>
@@ -4239,14 +4642,29 @@
     <row r="986" ht="15.75" customHeight="1">
       <c r="G986" s="5"/>
     </row>
+    <row r="987" ht="15.75" customHeight="1">
+      <c r="G987" s="5"/>
+    </row>
+    <row r="988" ht="15.75" customHeight="1">
+      <c r="G988" s="5"/>
+    </row>
+    <row r="989" ht="15.75" customHeight="1">
+      <c r="G989" s="5"/>
+    </row>
+    <row r="990" ht="15.75" customHeight="1">
+      <c r="G990" s="5"/>
+    </row>
+    <row r="991" ht="15.75" customHeight="1">
+      <c r="G991" s="5"/>
+    </row>
   </sheetData>
-  <autoFilter ref="$A$1:$J$27">
-    <sortState ref="A1:J27">
-      <sortCondition ref="E1:E27"/>
+  <autoFilter ref="$A$1:$J$32">
+    <sortState ref="A1:J32">
+      <sortCondition ref="E1:E32"/>
     </sortState>
   </autoFilter>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="G2:G986">
+    <dataValidation type="list" allowBlank="1" sqref="G2:G991">
       <formula1>"Yes,Maybe,No,Referral,Dead"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4280,34 +4698,34 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="8" t="s">
-        <v>62</v>
+      <c r="A1" s="10" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="9"/>
+      <c r="A2" s="11"/>
     </row>
     <row r="3">
-      <c r="A3" s="9" t="s">
-        <v>63</v>
+      <c r="A3" s="11" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="10" t="s">
-        <v>64</v>
+      <c r="A4" s="12" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="11"/>
+      <c r="A5" s="13"/>
     </row>
     <row r="6">
-      <c r="A6" s="11" t="s">
-        <v>65</v>
+      <c r="A6" s="13" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="12" t="s">
-        <v>66</v>
+      <c r="A7" s="14" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="8">
@@ -4318,15 +4736,15 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1"/>
     </row>
     <row r="12">
-      <c r="A12" s="13" t="s">
-        <v>68</v>
+      <c r="A12" s="15" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="13">
@@ -4334,49 +4752,49 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1"/>
     </row>
     <row r="16">
-      <c r="A16" s="14" t="s">
-        <v>70</v>
+      <c r="A16" s="16" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="13"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
     </row>
     <row r="18">
-      <c r="A18" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>72</v>
+      <c r="A18" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>76</v>
+      <c r="A19" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="20">
@@ -4384,12 +4802,12 @@
     </row>
     <row r="21" ht="15.0" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="16" t="s">
-        <v>78</v>
+      <c r="A22" s="18" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="23">
@@ -4406,7 +4824,7 @@
       <c r="A28" s="2"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="17"/>
+      <c r="A29" s="19"/>
     </row>
     <row r="30" ht="15.75" customHeight="1"/>
     <row r="31" ht="15.0" customHeight="1">
@@ -5400,6 +5818,400 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="33.71"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="22"/>
+      <c r="C2" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="22"/>
+      <c r="C3" s="7">
+        <v>2.0</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="22"/>
+      <c r="C4" s="7">
+        <v>3.0</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="22"/>
+      <c r="C5" s="7">
+        <v>4.0</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="22"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="22"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="23" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="24"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="25" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="26" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="26" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="26" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="26" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="26" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="26" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="22"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="21" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="27" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="28"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="29" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="28"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="28"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="29" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="27" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="28"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="29" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="28"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="29" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="28"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="29" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="28"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="29" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="28"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="28"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="28"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="21" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="29"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="29"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="29" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="27" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="28"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="29" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="28"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="28"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="27" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="27" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="28"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="29" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="28"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="28"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="27" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="27" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="28"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="29" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
   <sheetViews>
@@ -5412,7 +6224,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="6" t="s">
-        <v>79</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -6403,7 +7215,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <pageSetUpPr/>
@@ -6454,33 +7266,33 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>80</v>
+        <v>144</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>81</v>
+        <v>145</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>82</v>
+        <v>146</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>83</v>
+        <v>147</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>84</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>85</v>
+        <v>149</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -6489,67 +7301,72 @@
         <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>86</v>
+        <v>150</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>87</v>
+        <v>151</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>88</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>89</v>
+        <v>153</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>90</v>
+        <v>154</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>91</v>
+        <v>155</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>92</v>
+        <v>156</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" ht="15.0" customHeight="1">
       <c r="G6" s="1" t="s">
-        <v>93</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" ht="15.0" customHeight="1">
       <c r="G7" s="1" t="s">
-        <v>94</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" ht="15.0" customHeight="1">
       <c r="G8" s="1" t="s">
-        <v>95</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" ht="15.0" customHeight="1">
       <c r="G9" s="1" t="s">
-        <v>96</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" ht="15.0" customHeight="1">
       <c r="G10" s="1" t="s">
-        <v>97</v>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="E12" s="7" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Added MM logo transparent file
</commit_message>
<xml_diff>
--- a/docs/MindMirror_Marketing.xlsx
+++ b/docs/MindMirror_Marketing.xlsx
@@ -11,13 +11,13 @@
     <sheet state="visible" name="Sample" sheetId="6" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Outreach!$A$1:$J$32</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Outreach!$A$1:$J$36</definedName>
     <definedName hidden="1" localSheetId="5" name="_xlnm._FilterDatabase">Sample!$A$1:$H$4</definedName>
   </definedNames>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId10" roundtripDataChecksum="qzajpeeLuoBf6BjqMsoSghMdJ06MskDHULm3M8DAzp0="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId10" roundtripDataChecksum="MA8CVeVlqDEY25otkWaTyiL4ilxGbDI4tmFneTx8o8c="/>
     </ext>
   </extLst>
 </workbook>
@@ -71,6 +71,36 @@
 ======</t>
       </text>
     </comment>
+    <comment authorId="0" ref="G30">
+      <text>
+        <t xml:space="preserve">Proposed marketing services 
+======</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="E31">
+      <text>
+        <t xml:space="preserve">Building agents I believe, dev as well
+======</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="E32">
+      <text>
+        <t xml:space="preserve">Building similiar memory tools like me. Developer 
+======</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="E33">
+      <text>
+        <t xml:space="preserve">developer/builder, experimental mindset).
+======</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="E34">
+      <text>
+        <t xml:space="preserve">developer/builder, experimental mindset).
+======</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="G15">
       <text>
         <t xml:space="preserve">======
@@ -97,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="174">
   <si>
     <t>Name</t>
   </si>
@@ -298,6 +328,39 @@
   </si>
   <si>
     <t xml:space="preserve">Valekh </t>
+  </si>
+  <si>
+    <t>Dead</t>
+  </si>
+  <si>
+    <t>Creepy row Reddit user</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>Reddit</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/u/Creepy-Row970/s/aNTTqt6BhM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arindam </t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/u/Arindam_200/s/ee5HDJQIdz</t>
+  </si>
+  <si>
+    <t>Not ur buddy</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/u/Not_your_guy_buddy42/s/VTdOLkB1qa</t>
+  </si>
+  <si>
+    <t>Chisleu</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/u/chisleu/s/oW7M7aqnDr</t>
   </si>
   <si>
     <t>GPT lovers group</t>
@@ -742,7 +805,7 @@
     <numFmt numFmtId="164" formatCode="d\ mmm"/>
     <numFmt numFmtId="165" formatCode="d mmm"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -770,6 +833,10 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
     </font>
     <font>
       <b/>
@@ -863,7 +930,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -884,11 +951,14 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -898,34 +968,34 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -1750,47 +1820,122 @@
         <v>27</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="F30" s="9">
         <v>45948.0</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>57</v>
+        <v>67</v>
+      </c>
+      <c r="H30" s="9">
+        <v>45953.0</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="B31" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31" s="9">
+        <v>45952.0</v>
+      </c>
+      <c r="G31" s="5"/>
+    </row>
+    <row r="32" ht="15.75" customHeight="1">
+      <c r="A32" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" s="9">
+        <v>45953.0</v>
+      </c>
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" ht="15.75" customHeight="1">
+      <c r="A33" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" s="9">
+        <v>45953.0</v>
+      </c>
+      <c r="G33" s="5"/>
+    </row>
+    <row r="34" ht="15.75" customHeight="1">
+      <c r="A34" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" s="9">
+        <v>45953.0</v>
+      </c>
+      <c r="G34" s="5"/>
+    </row>
+    <row r="35" ht="15.75" customHeight="1">
+      <c r="A35" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E31" s="7" t="s">
+      <c r="E35" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="G31" s="5"/>
-    </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="G32" s="5"/>
-      <c r="J32" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="G33" s="5"/>
-    </row>
-    <row r="34" ht="15.75" customHeight="1">
-      <c r="G34" s="5"/>
-    </row>
-    <row r="35" ht="15.75" customHeight="1">
       <c r="G35" s="5"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="G36" s="5"/>
+      <c r="J36" s="2" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="G37" s="5"/>
@@ -4657,26 +4802,42 @@
     <row r="991" ht="15.75" customHeight="1">
       <c r="G991" s="5"/>
     </row>
+    <row r="992" ht="15.75" customHeight="1">
+      <c r="G992" s="5"/>
+    </row>
+    <row r="993" ht="15.75" customHeight="1">
+      <c r="G993" s="5"/>
+    </row>
+    <row r="994" ht="15.75" customHeight="1">
+      <c r="G994" s="5"/>
+    </row>
+    <row r="995" ht="15.75" customHeight="1">
+      <c r="G995" s="5"/>
+    </row>
   </sheetData>
-  <autoFilter ref="$A$1:$J$32">
-    <sortState ref="A1:J32">
-      <sortCondition ref="E1:E32"/>
+  <autoFilter ref="$A$1:$J$36">
+    <sortState ref="A1:J36">
+      <sortCondition ref="E1:E36"/>
     </sortState>
   </autoFilter>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="G2:G991">
+    <dataValidation type="list" allowBlank="1" sqref="G2:G995">
       <formula1>"Yes,Maybe,No,Referral,Dead"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink r:id="rId2" ref="D2"/>
     <hyperlink r:id="rId3" ref="D6"/>
+    <hyperlink r:id="rId4" ref="D31"/>
+    <hyperlink r:id="rId5" ref="D32"/>
+    <hyperlink r:id="rId6" ref="D33"/>
+    <hyperlink r:id="rId7" ref="D34"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="1.0" footer="0.0" header="0.0" left="0.75" right="0.75" top="1.0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId4"/>
-  <legacyDrawing r:id="rId5"/>
+  <drawing r:id="rId8"/>
+  <legacyDrawing r:id="rId9"/>
 </worksheet>
 </file>
 
@@ -4698,34 +4859,34 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="10" t="s">
-        <v>69</v>
+      <c r="A1" s="11" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="11"/>
+      <c r="A2" s="12"/>
     </row>
     <row r="3">
-      <c r="A3" s="11" t="s">
-        <v>70</v>
+      <c r="A3" s="12" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="12" t="s">
-        <v>71</v>
+      <c r="A4" s="13" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="13"/>
+      <c r="A5" s="14"/>
     </row>
     <row r="6">
-      <c r="A6" s="13" t="s">
-        <v>72</v>
+      <c r="A6" s="14" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="14" t="s">
-        <v>73</v>
+      <c r="A7" s="15" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="8">
@@ -4736,15 +4897,15 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1"/>
     </row>
     <row r="12">
-      <c r="A12" s="15" t="s">
-        <v>75</v>
+      <c r="A12" s="16" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="13">
@@ -4752,49 +4913,49 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1"/>
     </row>
     <row r="16">
-      <c r="A16" s="16" t="s">
-        <v>77</v>
+      <c r="A16" s="17" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="15"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
+      <c r="A17" s="16"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
     </row>
     <row r="18">
-      <c r="A18" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>79</v>
+      <c r="A18" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>83</v>
+      <c r="A19" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="20">
@@ -4802,12 +4963,12 @@
     </row>
     <row r="21" ht="15.0" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="18" t="s">
-        <v>85</v>
+      <c r="A22" s="19" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="23">
@@ -4824,7 +4985,7 @@
       <c r="A28" s="2"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="19"/>
+      <c r="A29" s="20"/>
     </row>
     <row r="30" ht="15.75" customHeight="1"/>
     <row r="31" ht="15.0" customHeight="1">
@@ -5828,209 +5989,209 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="C1" s="21" t="s">
-        <v>87</v>
+      <c r="A1" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="22"/>
+      <c r="A2" s="23"/>
       <c r="C2" s="7">
         <v>1.0</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="22"/>
+      <c r="A3" s="23"/>
       <c r="C3" s="7">
         <v>2.0</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="22"/>
+      <c r="A4" s="23"/>
       <c r="C4" s="7">
         <v>3.0</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="22"/>
+      <c r="A5" s="23"/>
       <c r="C5" s="7">
         <v>4.0</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="20" t="s">
-        <v>92</v>
+      <c r="A6" s="21" t="s">
+        <v>103</v>
       </c>
       <c r="C6" s="7">
         <v>5.0</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="22"/>
+      <c r="A7" s="23"/>
     </row>
     <row r="8">
-      <c r="A8" s="22"/>
+      <c r="A8" s="23"/>
     </row>
     <row r="9">
-      <c r="A9" s="23" t="s">
-        <v>94</v>
+      <c r="A9" s="24" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="24"/>
+      <c r="A10" s="25"/>
     </row>
     <row r="11">
-      <c r="A11" s="25" t="s">
-        <v>95</v>
+      <c r="A11" s="26" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="26" t="s">
-        <v>96</v>
+      <c r="A12" s="27" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="26" t="s">
-        <v>97</v>
+      <c r="A13" s="27" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="26" t="s">
-        <v>98</v>
+      <c r="A14" s="27" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="26" t="s">
-        <v>99</v>
+      <c r="A15" s="27" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="26" t="s">
-        <v>100</v>
+      <c r="A16" s="27" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="26" t="s">
-        <v>101</v>
+      <c r="A17" s="27" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="22"/>
+      <c r="A20" s="23"/>
     </row>
     <row r="22">
-      <c r="A22" s="21" t="s">
-        <v>102</v>
+      <c r="A22" s="22" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="7" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="7" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="7" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="7" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="7" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="7" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="7" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="7" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -6049,158 +6210,158 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="27" t="s">
-        <v>123</v>
+      <c r="A1" s="28" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="28"/>
+      <c r="A2" s="29"/>
     </row>
     <row r="3">
-      <c r="A3" s="29" t="s">
-        <v>124</v>
+      <c r="A3" s="30" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="28"/>
+      <c r="A4" s="29"/>
     </row>
     <row r="6">
-      <c r="A6" s="28"/>
+      <c r="A6" s="29"/>
     </row>
     <row r="7">
-      <c r="A7" s="29" t="s">
-        <v>125</v>
+      <c r="A7" s="30" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="27" t="s">
-        <v>126</v>
+      <c r="A8" s="28" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="28"/>
+      <c r="A9" s="29"/>
     </row>
     <row r="10">
-      <c r="A10" s="29" t="s">
-        <v>127</v>
+      <c r="A10" s="30" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="28"/>
+      <c r="A11" s="29"/>
     </row>
     <row r="12">
-      <c r="A12" s="29" t="s">
-        <v>128</v>
+      <c r="A12" s="30" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="28"/>
+      <c r="A13" s="29"/>
     </row>
     <row r="14">
-      <c r="A14" s="29" t="s">
-        <v>129</v>
+      <c r="A14" s="30" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="28"/>
+      <c r="A15" s="29"/>
     </row>
     <row r="16">
-      <c r="A16" s="29" t="s">
-        <v>130</v>
+      <c r="A16" s="30" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="28"/>
+      <c r="A17" s="29"/>
     </row>
     <row r="18">
-      <c r="A18" s="28"/>
+      <c r="A18" s="29"/>
     </row>
     <row r="19">
-      <c r="A19" s="28"/>
+      <c r="A19" s="29"/>
     </row>
     <row r="20">
-      <c r="A20" s="21" t="s">
-        <v>131</v>
+      <c r="A20" s="22" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="23" t="s">
-        <v>132</v>
+      <c r="A21" s="24" t="s">
+        <v>143</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="29"/>
+      <c r="A22" s="30"/>
     </row>
     <row r="23">
-      <c r="A23" s="29"/>
+      <c r="A23" s="30"/>
     </row>
     <row r="24">
-      <c r="A24" s="29" t="s">
-        <v>134</v>
+      <c r="A24" s="30" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="27" t="s">
-        <v>135</v>
+      <c r="A25" s="28" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="28"/>
+      <c r="A26" s="29"/>
     </row>
     <row r="27">
-      <c r="A27" s="29" t="s">
-        <v>136</v>
+      <c r="A27" s="30" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="28"/>
+      <c r="A28" s="29"/>
     </row>
     <row r="30">
-      <c r="A30" s="28"/>
+      <c r="A30" s="29"/>
     </row>
     <row r="31">
-      <c r="A31" s="27" t="s">
-        <v>137</v>
+      <c r="A31" s="28" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="27" t="s">
-        <v>138</v>
+      <c r="A32" s="28" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="28"/>
+      <c r="A33" s="29"/>
     </row>
     <row r="34">
-      <c r="A34" s="29" t="s">
-        <v>139</v>
+      <c r="A34" s="30" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="28"/>
+      <c r="A35" s="29"/>
     </row>
     <row r="37">
-      <c r="A37" s="28"/>
+      <c r="A37" s="29"/>
     </row>
     <row r="38">
-      <c r="A38" s="27" t="s">
-        <v>140</v>
+      <c r="A38" s="28" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="27" t="s">
-        <v>141</v>
+      <c r="A39" s="28" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="28"/>
+      <c r="A40" s="29"/>
     </row>
     <row r="41">
-      <c r="A41" s="29" t="s">
-        <v>142</v>
+      <c r="A41" s="30" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -6224,7 +6385,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="6" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -7266,7 +7427,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>60</v>
@@ -7275,24 +7436,24 @@
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -7301,39 +7462,39 @@
         <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>45</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>57</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>38</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>43</v>
@@ -7341,32 +7502,32 @@
     </row>
     <row r="6" ht="15.0" customHeight="1">
       <c r="G6" s="1" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" ht="15.0" customHeight="1">
       <c r="G7" s="1" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" ht="15.0" customHeight="1">
       <c r="G8" s="1" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" ht="15.0" customHeight="1">
       <c r="G9" s="1" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" ht="15.0" customHeight="1">
       <c r="G10" s="1" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
     </row>
     <row r="12">
       <c r="E12" s="7" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Update homepage and about page videos
- Changed homepage video to new YouTube demo (Yv9zTDUaVdg)
- Removed video section from about page
- Added YouTube channel link to about page social links
- Updated video container to full-width 16:9 format

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/docs/MindMirror_Marketing.xlsx
+++ b/docs/MindMirror_Marketing.xlsx
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="174">
   <si>
     <t>Name</t>
   </si>
@@ -1595,7 +1595,9 @@
       <c r="F18" s="4">
         <v>45940.0</v>
       </c>
-      <c r="G18" s="5"/>
+      <c r="G18" s="7" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="2" t="s">

</xml_diff>

<commit_message>
Enhance Windsurf integration page and fix code block scrolling
**Windsurf Integration Improvements:**
- Add comprehensive Windsurf MCP config setup guide with step-by-step UI navigation
- Include detailed instructions for accessing MCP panel through Windsurf logo → Cascade → MCP Marketplace
- Add collapsible troubleshooting section with Accordion component:
  - npx PATH configuration solutions
  - Connection hang fixes
  - Terminal testing command for debugging
- Update config to include -y flag to prevent npx install prompts
- Fix URL consistency: memory.usemindmirror.com across all integration pages

**Code Block Formatting Fixes:**
- Integration.tsx: Fixed all pre/code blocks to use whitespace-pre and whitespace-nowrap
- HeroSection.tsx: Added whitespace-nowrap to URL preview
- TokenModal.tsx: Added overflow-x-auto to token and URL input fields

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/docs/MindMirror_Marketing.xlsx
+++ b/docs/MindMirror_Marketing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Programming_Projects/MCP_Memory/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0113BE97-1630-AE4D-AB72-432B9AA05754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{681A0920-9AA8-4C44-AA7C-229676A9109B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2160" yWindow="840" windowWidth="27920" windowHeight="17160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -169,15 +169,41 @@
         <r>
           <rPr>
             <sz val="11"/>
-            <color theme="1"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
-          <t>======
-ID#AAABsCcTdwg
-None    (2025-10-10 13:10:39)
-should try in next couple days and lmk what he thinks might try with Cursor</t>
+          <t xml:space="preserve">======
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">ID#AAABsCcTdwg
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">None    (2025-10-10 13:10:39)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>should try in next couple days and lmk what he thinks might try with Cursor</t>
         </r>
       </text>
     </comment>
@@ -1152,9 +1178,6 @@
     <t>High – emotional AI companion with long-term context</t>
   </si>
   <si>
-    <t>Sent email + LinkedIn request. Optional PH comment.https://www.linkedin.com/in/alirezabeig</t>
-  </si>
-  <si>
     <t>High – AI therapy with long-term mood and chat history</t>
   </si>
   <si>
@@ -1239,6 +1262,9 @@
   </si>
   <si>
     <t xml:space="preserve">Tier A - Solo dev (Gary Sabo), email sent, Reddit DM to wife (u/jac_myndarc), Twitter reply to @GarySabo on feature update thread. 3 channels hit. LinkedIn skipped (connection limit). </t>
+  </si>
+  <si>
+    <t>Sent email + LinkedIn request. Optional PH comment.https://www.linkedin.com/in/alirezabeig Alireza responded to linked in personalized connection request  San Francisco, emotional AI companion (Pal), accepted connection, sent full pitch with demo link |</t>
   </si>
 </sst>
 </file>
@@ -1413,7 +1439,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1444,6 +1470,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1664,8 +1691,8 @@
   <dimension ref="A1:K997"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F65" sqref="F65"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1907,7 +1934,9 @@
       <c r="E11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="4"/>
+      <c r="F11" s="4">
+        <v>45982</v>
+      </c>
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -1941,7 +1970,13 @@
       <c r="E13" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="F13" s="26">
+        <v>45940</v>
+      </c>
       <c r="G13" s="5"/>
+      <c r="H13" s="26">
+        <v>45982</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
@@ -1991,7 +2026,9 @@
       <c r="E16" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F16" s="4"/>
+      <c r="F16" s="4">
+        <v>45981</v>
+      </c>
       <c r="G16" s="5"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -2213,7 +2250,7 @@
         <v>58</v>
       </c>
       <c r="H27" s="4">
-        <v>45949</v>
+        <v>45982</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2236,6 +2273,9 @@
         <v>45946</v>
       </c>
       <c r="G28" s="5"/>
+      <c r="H28" s="26">
+        <v>45981</v>
+      </c>
     </row>
     <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
@@ -2519,11 +2559,11 @@
         <v>261</v>
       </c>
       <c r="F41" s="6">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="G41" s="5"/>
       <c r="I41" s="5" t="s">
-        <v>262</v>
+        <v>286</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2537,31 +2577,31 @@
         <v>80</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E42" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F42" s="6">
         <v>45980</v>
       </c>
       <c r="G42" s="5"/>
       <c r="I42" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="B43" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="B43" s="5" t="s">
-        <v>266</v>
-      </c>
       <c r="C43" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>12</v>
@@ -2571,7 +2611,7 @@
         <v>96</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -2591,13 +2631,13 @@
         <v>100</v>
       </c>
       <c r="F44" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="G44" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="G44" s="5" t="s">
+      <c r="I44" s="14" t="s">
         <v>271</v>
-      </c>
-      <c r="I44" s="14" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -2618,10 +2658,10 @@
       </c>
       <c r="F45" s="6"/>
       <c r="G45" s="5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I45" s="14" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -2642,10 +2682,10 @@
       </c>
       <c r="F46" s="6"/>
       <c r="G46" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="I46" s="14" t="s">
         <v>274</v>
-      </c>
-      <c r="I46" s="14" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
@@ -2666,10 +2706,10 @@
       </c>
       <c r="F47" s="6"/>
       <c r="G47" s="5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I47" s="25" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
@@ -2704,7 +2744,7 @@
         <v>80</v>
       </c>
       <c r="D49" s="25" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E49" t="s">
         <v>94</v>
@@ -2714,7 +2754,7 @@
       </c>
       <c r="G49" s="5"/>
       <c r="I49" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -2728,17 +2768,17 @@
         <v>80</v>
       </c>
       <c r="D50" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E50" t="s">
         <v>114</v>
       </c>
       <c r="F50" s="6"/>
       <c r="G50" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I50" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -2759,10 +2799,10 @@
       </c>
       <c r="F51" s="6"/>
       <c r="G51" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -2806,10 +2846,10 @@
         <v>45972.596344965277</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I53" s="24" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -2832,10 +2872,10 @@
         <v>45972.596344965277</v>
       </c>
       <c r="G54" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="I54" s="5" t="s">
         <v>283</v>
-      </c>
-      <c r="I54" s="5" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -2858,10 +2898,10 @@
         <v>45972.596344965277</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2885,7 +2925,7 @@
       </c>
       <c r="G56" s="5"/>
       <c r="I56" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>